<commit_message>
Updated to Class Methods
Deleted Text Files
</commit_message>
<xml_diff>
--- a/Handicap Index Course Handicap Report.xlsx
+++ b/Handicap Index Course Handicap Report.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="0" windowWidth="14960" windowHeight="17600"/>
+    <workbookView xWindow="360" yWindow="280" windowWidth="14940" windowHeight="12920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
   <si>
     <t>GHIN #</t>
   </si>
@@ -168,7 +168,7 @@
     <t>Bob Heard</t>
   </si>
   <si>
-    <t>6.1</t>
+    <t>6.2</t>
   </si>
   <si>
     <t>6</t>
@@ -198,7 +198,10 @@
     <t>Jim Sido</t>
   </si>
   <si>
-    <t>10.4</t>
+    <t>10.7</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
   <si>
     <t>Stewart</t>
@@ -219,9 +222,6 @@
     <t>11.6</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>Traub</t>
   </si>
   <si>
@@ -240,7 +240,10 @@
     <t>Al Vela</t>
   </si>
   <si>
-    <t>19.1</t>
+    <t>19.0</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
   <si>
     <t>25</t>
@@ -1046,7 +1049,7 @@
         <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>17</v>
@@ -1149,10 +1152,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>36</v>
@@ -1165,13 +1168,13 @@
         <v>7701708</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>36</v>
@@ -1190,16 +1193,16 @@
         <v>53161</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>11</v>
@@ -1252,10 +1255,10 @@
         <v>18</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1265,13 +1268,13 @@
         <v>3661053</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>12</v>
@@ -1290,29 +1293,29 @@
         <v>3661061</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" ht="17" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C21" s="9">
         <v>19</v>
@@ -1320,7 +1323,7 @@
     </row>
     <row r="22" spans="1:9" ht="17" customHeight="1">
       <c r="A22" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B22" s="13">
         <v>1</v>
@@ -1328,10 +1331,10 @@
     </row>
     <row r="23" spans="1:9" ht="17" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C23" s="11">
-        <v>43874.167361111111</v>
+        <v>43877.167361111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for Road Trip hcp/slope/rtg
</commit_message>
<xml_diff>
--- a/Handicap Index Course Handicap Report.xlsx
+++ b/Handicap Index Course Handicap Report.xlsx
@@ -37,163 +37,166 @@
     <t>Reid Baker</t>
   </si>
   <si>
-    <t>11.4</t>
+    <t>11.8</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Barnard</t>
+  </si>
+  <si>
+    <t>Bill Barnard</t>
+  </si>
+  <si>
+    <t>16.7</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Baumgarth</t>
+  </si>
+  <si>
+    <t>Rick Baumgarth</t>
+  </si>
+  <si>
+    <t>11.7</t>
+  </si>
+  <si>
+    <t>Besse</t>
+  </si>
+  <si>
+    <t>Rick Besse</t>
+  </si>
+  <si>
+    <t>15.2</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Broyles</t>
+  </si>
+  <si>
+    <t>Frank Broyles</t>
+  </si>
+  <si>
+    <t>15.4</t>
+  </si>
+  <si>
+    <t>Carroll</t>
+  </si>
+  <si>
+    <t>Jack Carroll</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Barnard</t>
-  </si>
-  <si>
-    <t>Bill Barnard</t>
-  </si>
-  <si>
-    <t>16.5</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Baumgarth</t>
-  </si>
-  <si>
-    <t>Rick Baumgarth</t>
-  </si>
-  <si>
-    <t>Besse</t>
-  </si>
-  <si>
-    <t>Rick Besse</t>
-  </si>
-  <si>
-    <t>16.1</t>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Will Davis</t>
+  </si>
+  <si>
+    <t>14.5</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Duron</t>
+  </si>
+  <si>
+    <t>Rocky Duron</t>
+  </si>
+  <si>
+    <t>16.2</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>Broyles</t>
-  </si>
-  <si>
-    <t>Frank Broyles</t>
-  </si>
-  <si>
-    <t>15.5</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Carroll</t>
-  </si>
-  <si>
-    <t>Jack Carroll</t>
-  </si>
-  <si>
-    <t>10.0</t>
+    <t>Fannon</t>
+  </si>
+  <si>
+    <t>Kent Fannon</t>
+  </si>
+  <si>
+    <t>13.9</t>
+  </si>
+  <si>
+    <t>Fitzgerald</t>
+  </si>
+  <si>
+    <t>Curt Fitzgerald</t>
+  </si>
+  <si>
+    <t>16.9</t>
+  </si>
+  <si>
+    <t>Heard</t>
+  </si>
+  <si>
+    <t>Bob Heard</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Humphrey</t>
+  </si>
+  <si>
+    <t>Richard Humphrey</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Sido</t>
+  </si>
+  <si>
+    <t>Jim Sido</t>
+  </si>
+  <si>
+    <t>8.2</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Davis</t>
-  </si>
-  <si>
-    <t>Will Davis</t>
-  </si>
-  <si>
-    <t>15.6</t>
-  </si>
-  <si>
-    <t>Duron</t>
-  </si>
-  <si>
-    <t>Rocky Duron</t>
-  </si>
-  <si>
-    <t>16.2</t>
-  </si>
-  <si>
-    <t>Fannon</t>
-  </si>
-  <si>
-    <t>Kent Fannon</t>
-  </si>
-  <si>
-    <t>15.2</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Fitzgerald</t>
-  </si>
-  <si>
-    <t>Curt Fitzgerald</t>
-  </si>
-  <si>
-    <t>18.2</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Heard</t>
-  </si>
-  <si>
-    <t>Bob Heard</t>
-  </si>
-  <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Humphrey</t>
-  </si>
-  <si>
-    <t>Richard Humphrey</t>
-  </si>
-  <si>
-    <t>17.6</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Sido</t>
-  </si>
-  <si>
-    <t>Jim Sido</t>
-  </si>
-  <si>
-    <t>10.6</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>Stewart</t>
   </si>
   <si>
     <t>Dan Stewart</t>
   </si>
   <si>
-    <t>13.2</t>
+    <t>10.3</t>
   </si>
   <si>
     <t>Strand</t>
@@ -202,7 +205,7 @@
     <t>Bill  Strand</t>
   </si>
   <si>
-    <t>11.2</t>
+    <t>9.9</t>
   </si>
   <si>
     <t>Traub</t>
@@ -211,10 +214,7 @@
     <t>Larry Traub</t>
   </si>
   <si>
-    <t>8.9</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>8.5</t>
   </si>
   <si>
     <t>Vela</t>
@@ -223,7 +223,7 @@
     <t>Al Vela</t>
   </si>
   <si>
-    <t>19.5</t>
+    <t>19.4</t>
   </si>
   <si>
     <t>23</t>
@@ -238,16 +238,13 @@
     <t>14.9</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Williams</t>
   </si>
   <si>
     <t>Doug Williams</t>
   </si>
   <si>
-    <t>18.9</t>
+    <t>17.0</t>
   </si>
   <si>
     <t>Total Golfers:</t>
@@ -267,15 +264,15 @@
     <numFmt numFmtId="50" formatCode="####0"/>
     <numFmt numFmtId="51" formatCode="M/d/yyyy h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="9.0"/>
       <name val="Arial"/>
-      <color rgb="ff3f3f3f"/>
+      <color rgb="ffffffff"/>
       <b/>
       <u val="single"/>
     </font>
@@ -284,19 +281,8 @@
       <name val="Arial"/>
       <color rgb="ff3f3f3f"/>
     </font>
-    <font>
-      <sz val="7.0"/>
-      <name val="Arial"/>
-      <color rgb="ff3f3f3f"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="7.0"/>
-      <name val="Arial"/>
-      <color rgb="ff3f3f3f"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -305,12 +291,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="ffffffff"/>
+        <fgColor rgb="ff4278b3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="fff5f5f5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ffffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -350,7 +341,7 @@
       </bottom>
     </border>
   </borders>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf/>
     <xf fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" horizontal="center" wrapText="1"/>
@@ -367,28 +358,22 @@
     <xf fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="50" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="50" applyNumberFormat="1" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="50" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="50" applyNumberFormat="1" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf numFmtId="51" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" horizontal="left"/>
-    </xf>
-    <xf fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" horizontal="left"/>
-    </xf>
-    <xf numFmtId="50" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="51" applyNumberFormat="1" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
   </cellXfs>
@@ -399,21 +384,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <cols>
     <col min="1" max="1" width="55.04761904761905" customWidth="1"/>
-    <col min="2" max="2" width="16.0" customWidth="1"/>
+    <col min="2" max="2" width="14.476190476190476" customWidth="1"/>
     <col min="3" max="3" width="40.38095238095238" customWidth="1"/>
-    <col min="4" max="4" width="4.380952380952381" customWidth="1"/>
-    <col min="5" max="5" width="12.571428571428571" customWidth="1"/>
+    <col min="4" max="4" width="35.42857142857143" customWidth="1"/>
+    <col min="5" max="5" width="4.380952380952381" customWidth="1"/>
     <col min="6" max="6" width="12.571428571428571" customWidth="1"/>
     <col min="7" max="7" width="12.571428571428571" customWidth="1"/>
     <col min="8" max="8" width="12.571428571428571" customWidth="1"/>
     <col min="9" max="9" width="12.571428571428571" customWidth="1"/>
+    <col min="10" max="10" width="12.571428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c s="2" t="s">
@@ -436,7 +422,7 @@
       <c r="A2" s="3">
         <v>3660253.0</v>
       </c>
-      <c s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c s="4" t="s">
@@ -459,7 +445,7 @@
       <c r="A3" s="6">
         <v>5910694.0</v>
       </c>
-      <c s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
       <c s="7" t="s">
@@ -482,14 +468,14 @@
       <c r="A4" s="3">
         <v>3660265.0</v>
       </c>
-      <c s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
       <c s="4" t="s">
         <v>17</v>
       </c>
       <c s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c s="5" t="s">
         <v>9</v>
@@ -505,20 +491,20 @@
       <c r="A5" s="6">
         <v>3660283.0</v>
       </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
       <c s="7" t="s">
-        <v>18</v>
-      </c>
-      <c s="7" t="s">
-        <v>19</v>
-      </c>
-      <c s="8" t="s">
         <v>20</v>
       </c>
       <c s="8" t="s">
-        <v>14</v>
-      </c>
-      <c s="8" t="s">
         <v>21</v>
+      </c>
+      <c s="8" t="s">
+        <v>22</v>
+      </c>
+      <c s="8" t="s">
+        <v>23</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -528,20 +514,20 @@
       <c r="A6" s="3">
         <v>2379621.0</v>
       </c>
-      <c s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c s="4" t="s">
+        <v>25</v>
+      </c>
+      <c s="5" t="s">
+        <v>26</v>
+      </c>
+      <c s="5" t="s">
         <v>22</v>
       </c>
-      <c s="4" t="s">
+      <c s="5" t="s">
         <v>23</v>
-      </c>
-      <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5" t="s">
-        <v>25</v>
-      </c>
-      <c s="5" t="s">
-        <v>21</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -551,13 +537,10 @@
       <c r="A7" s="6">
         <v>3660366.0</v>
       </c>
+      <c r="C7" s="7" t="s">
+        <v>27</v>
+      </c>
       <c s="7" t="s">
-        <v>26</v>
-      </c>
-      <c s="7" t="s">
-        <v>27</v>
-      </c>
-      <c s="8" t="s">
         <v>28</v>
       </c>
       <c s="8" t="s">
@@ -565,6 +548,9 @@
       </c>
       <c s="8" t="s">
         <v>30</v>
+      </c>
+      <c s="8" t="s">
+        <v>31</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -574,20 +560,20 @@
       <c r="A8" s="3">
         <v>1815996.0</v>
       </c>
-      <c s="4" t="s">
-        <v>31</v>
-      </c>
-      <c s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>32</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>33</v>
       </c>
       <c s="5" t="s">
-        <v>25</v>
-      </c>
-      <c s="5" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c s="5" t="s">
+        <v>35</v>
+      </c>
+      <c s="5" t="s">
+        <v>14</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -597,20 +583,20 @@
       <c r="A9" s="6">
         <v>3720105.0</v>
       </c>
+      <c r="C9" s="7" t="s">
+        <v>36</v>
+      </c>
       <c s="7" t="s">
-        <v>34</v>
-      </c>
-      <c s="7" t="s">
-        <v>35</v>
-      </c>
-      <c s="8" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c s="8" t="s">
+        <v>38</v>
       </c>
       <c s="8" t="s">
         <v>14</v>
       </c>
       <c s="8" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -620,20 +606,20 @@
       <c r="A10" s="3">
         <v>3660486.0</v>
       </c>
-      <c s="4" t="s">
-        <v>37</v>
-      </c>
-      <c s="4" t="s">
-        <v>38</v>
-      </c>
-      <c s="5" t="s">
-        <v>39</v>
-      </c>
-      <c s="5" t="s">
-        <v>25</v>
-      </c>
-      <c s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>40</v>
+      </c>
+      <c s="4" t="s">
+        <v>41</v>
+      </c>
+      <c s="5" t="s">
+        <v>42</v>
+      </c>
+      <c s="5" t="s">
+        <v>10</v>
+      </c>
+      <c s="5" t="s">
+        <v>14</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -643,20 +629,20 @@
       <c r="A11" s="6">
         <v>2379581.0</v>
       </c>
+      <c r="C11" s="7" t="s">
+        <v>43</v>
+      </c>
       <c s="7" t="s">
-        <v>41</v>
-      </c>
-      <c s="7" t="s">
-        <v>42</v>
-      </c>
-      <c s="8" t="s">
-        <v>43</v>
-      </c>
-      <c s="8" t="s">
-        <v>21</v>
-      </c>
-      <c s="8" t="s">
         <v>44</v>
+      </c>
+      <c s="8" t="s">
+        <v>45</v>
+      </c>
+      <c s="8" t="s">
+        <v>14</v>
+      </c>
+      <c s="8" t="s">
+        <v>15</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -666,13 +652,10 @@
       <c r="A12" s="3">
         <v>3660603.0</v>
       </c>
-      <c s="4" t="s">
-        <v>45</v>
-      </c>
-      <c s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>46</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>47</v>
       </c>
       <c s="5" t="s">
@@ -680,6 +663,9 @@
       </c>
       <c s="5" t="s">
         <v>49</v>
+      </c>
+      <c s="5" t="s">
+        <v>50</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -689,20 +675,20 @@
       <c r="A13" s="6">
         <v>3660992.0</v>
       </c>
+      <c r="C13" s="7" t="s">
+        <v>51</v>
+      </c>
       <c s="7" t="s">
-        <v>50</v>
-      </c>
-      <c s="7" t="s">
-        <v>51</v>
-      </c>
-      <c s="8" t="s">
         <v>52</v>
       </c>
       <c s="8" t="s">
-        <v>40</v>
-      </c>
-      <c s="8" t="s">
         <v>53</v>
+      </c>
+      <c s="8" t="s">
+        <v>39</v>
+      </c>
+      <c s="8" t="s">
+        <v>54</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -712,20 +698,20 @@
       <c r="A14" s="3">
         <v>4787165.0</v>
       </c>
-      <c s="4" t="s">
-        <v>54</v>
-      </c>
-      <c s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>55</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>56</v>
       </c>
       <c s="5" t="s">
-        <v>29</v>
-      </c>
-      <c s="5" t="s">
         <v>57</v>
+      </c>
+      <c s="5" t="s">
+        <v>50</v>
+      </c>
+      <c s="5" t="s">
+        <v>58</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -735,20 +721,20 @@
       <c r="A15" s="6">
         <v>7701708.0</v>
       </c>
+      <c r="C15" s="7" t="s">
+        <v>59</v>
+      </c>
       <c s="7" t="s">
+        <v>60</v>
+      </c>
+      <c s="8" t="s">
+        <v>61</v>
+      </c>
+      <c s="8" t="s">
         <v>58</v>
       </c>
-      <c s="7" t="s">
-        <v>59</v>
-      </c>
-      <c s="8" t="s">
-        <v>60</v>
-      </c>
-      <c s="8" t="s">
-        <v>57</v>
-      </c>
-      <c s="8" t="s">
-        <v>25</v>
+      <c s="8" t="s">
+        <v>9</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -758,20 +744,20 @@
       <c r="A16" s="3">
         <v>53161.0</v>
       </c>
-      <c s="4" t="s">
-        <v>61</v>
-      </c>
-      <c s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>62</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>63</v>
       </c>
       <c s="5" t="s">
+        <v>64</v>
+      </c>
+      <c s="5" t="s">
+        <v>58</v>
+      </c>
+      <c s="5" t="s">
         <v>9</v>
-      </c>
-      <c s="5" t="s">
-        <v>57</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -781,20 +767,20 @@
       <c r="A17" s="6">
         <v>4548474.0</v>
       </c>
+      <c r="C17" s="7" t="s">
+        <v>65</v>
+      </c>
       <c s="7" t="s">
-        <v>64</v>
-      </c>
-      <c s="7" t="s">
-        <v>65</v>
-      </c>
-      <c s="8" t="s">
         <v>66</v>
       </c>
       <c s="8" t="s">
         <v>67</v>
       </c>
       <c s="8" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c s="8" t="s">
+        <v>58</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -804,7 +790,7 @@
       <c r="A18" s="3">
         <v>3661029.0</v>
       </c>
-      <c s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>68</v>
       </c>
       <c s="4" t="s">
@@ -827,7 +813,7 @@
       <c r="A19" s="6">
         <v>3661053.0</v>
       </c>
-      <c s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>72</v>
       </c>
       <c s="7" t="s">
@@ -837,10 +823,10 @@
         <v>74</v>
       </c>
       <c s="8" t="s">
-        <v>75</v>
-      </c>
-      <c s="8" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c s="8" t="s">
+        <v>23</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -850,20 +836,20 @@
       <c r="A20" s="3">
         <v>3661061.0</v>
       </c>
+      <c r="C20" s="4" t="s">
+        <v>75</v>
+      </c>
       <c s="4" t="s">
         <v>76</v>
       </c>
-      <c s="4" t="s">
+      <c s="5" t="s">
         <v>77</v>
       </c>
       <c s="5" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c s="5" t="s">
         <v>15</v>
-      </c>
-      <c s="5" t="s">
-        <v>44</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -871,26 +857,26 @@
     </row>
     <row r="21" ht="17.0" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="9">
         <v>19.0</v>
       </c>
     </row>
     <row r="22" ht="17.0" customHeight="1">
-      <c r="A22" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c s="13">
+      <c r="A22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c s="9">
         <v>1.0</v>
       </c>
     </row>
     <row r="23" ht="17.0" customHeight="1">
-      <c r="A23" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="11">
-        <v>43926.125023148146</v>
+      <c r="A23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="11">
+        <v>43959.12503472222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Handicap Index Course Handicap Report.xlsx
</commit_message>
<xml_diff>
--- a/Handicap Index Course Handicap Report.xlsx
+++ b/Handicap Index Course Handicap Report.xlsx
@@ -115,7 +115,7 @@
     <t>Will Davis</t>
   </si>
   <si>
-    <t>14.5</t>
+    <t>14.7</t>
   </si>
   <si>
     <t>15</t>
@@ -139,7 +139,10 @@
     <t>Kent Fannon</t>
   </si>
   <si>
-    <t>13.9</t>
+    <t>13.4</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
   <si>
     <t>Fitzgerald</t>
@@ -205,7 +208,7 @@
     <t>Bill  Strand</t>
   </si>
   <si>
-    <t>9.9</t>
+    <t>9.8</t>
   </si>
   <si>
     <t>Traub</t>
@@ -244,7 +247,7 @@
     <t>Doug Williams</t>
   </si>
   <si>
-    <t>17.0</t>
+    <t>17.1</t>
   </si>
   <si>
     <t>Total Golfers:</t>
@@ -264,15 +267,15 @@
     <numFmt numFmtId="50" formatCode="####0"/>
     <numFmt numFmtId="51" formatCode="M/d/yyyy h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="10.0"/>
       <name val="Arial"/>
-      <color rgb="ffffffff"/>
+      <color rgb="ff3f3f3f"/>
       <b/>
       <u val="single"/>
     </font>
@@ -281,8 +284,19 @@
       <name val="Arial"/>
       <color rgb="ff3f3f3f"/>
     </font>
+    <font>
+      <sz val="7.0"/>
+      <name val="Arial"/>
+      <color rgb="ff3f3f3f"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="7.0"/>
+      <name val="Arial"/>
+      <color rgb="ff3f3f3f"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -291,17 +305,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="ff4278b3"/>
+        <fgColor rgb="ffffffff"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="fff5f5f5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ffffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -341,7 +350,7 @@
       </bottom>
     </border>
   </borders>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf/>
     <xf fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" horizontal="center" wrapText="1"/>
@@ -358,22 +367,28 @@
     <xf fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="50" applyNumberFormat="1" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="50" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="center"/>
     </xf>
-    <xf numFmtId="50" applyNumberFormat="1" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="50" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
+    <xf fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf numFmtId="51" applyNumberFormat="1" fontId="2" applyFont="1" fillId="4" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="51" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" horizontal="left"/>
+    </xf>
+    <xf fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" horizontal="left"/>
+    </xf>
+    <xf numFmtId="50" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" horizontal="left"/>
     </xf>
   </cellXfs>
@@ -384,22 +399,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <cols>
     <col min="1" max="1" width="55.04761904761905" customWidth="1"/>
-    <col min="2" max="2" width="14.476190476190476" customWidth="1"/>
+    <col min="2" max="2" width="16.0" customWidth="1"/>
     <col min="3" max="3" width="40.38095238095238" customWidth="1"/>
-    <col min="4" max="4" width="35.42857142857143" customWidth="1"/>
-    <col min="5" max="5" width="4.380952380952381" customWidth="1"/>
+    <col min="4" max="4" width="4.380952380952381" customWidth="1"/>
+    <col min="5" max="5" width="12.571428571428571" customWidth="1"/>
     <col min="6" max="6" width="12.571428571428571" customWidth="1"/>
     <col min="7" max="7" width="12.571428571428571" customWidth="1"/>
     <col min="8" max="8" width="12.571428571428571" customWidth="1"/>
     <col min="9" max="9" width="12.571428571428571" customWidth="1"/>
-    <col min="10" max="10" width="12.571428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c s="2" t="s">
         <v>1</v>
       </c>
       <c s="2" t="s">
@@ -422,7 +436,7 @@
       <c r="A2" s="3">
         <v>3660253.0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c s="4" t="s">
         <v>6</v>
       </c>
       <c s="4" t="s">
@@ -445,7 +459,7 @@
       <c r="A3" s="6">
         <v>5910694.0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c s="7" t="s">
         <v>11</v>
       </c>
       <c s="7" t="s">
@@ -468,7 +482,7 @@
       <c r="A4" s="3">
         <v>3660265.0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c s="4" t="s">
         <v>16</v>
       </c>
       <c s="4" t="s">
@@ -491,7 +505,7 @@
       <c r="A5" s="6">
         <v>3660283.0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c s="7" t="s">
         <v>19</v>
       </c>
       <c s="7" t="s">
@@ -514,7 +528,7 @@
       <c r="A6" s="3">
         <v>2379621.0</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c s="4" t="s">
         <v>24</v>
       </c>
       <c s="4" t="s">
@@ -537,7 +551,7 @@
       <c r="A7" s="6">
         <v>3660366.0</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c s="7" t="s">
         <v>27</v>
       </c>
       <c s="7" t="s">
@@ -560,7 +574,7 @@
       <c r="A8" s="3">
         <v>1815996.0</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c s="4" t="s">
         <v>32</v>
       </c>
       <c s="4" t="s">
@@ -573,7 +587,7 @@
         <v>35</v>
       </c>
       <c s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -583,7 +597,7 @@
       <c r="A9" s="6">
         <v>3720105.0</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c s="7" t="s">
         <v>36</v>
       </c>
       <c s="7" t="s">
@@ -606,7 +620,7 @@
       <c r="A10" s="3">
         <v>3660486.0</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c s="4" t="s">
         <v>40</v>
       </c>
       <c s="4" t="s">
@@ -616,10 +630,10 @@
         <v>42</v>
       </c>
       <c s="5" t="s">
-        <v>10</v>
-      </c>
-      <c s="5" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c s="5" t="s">
+        <v>22</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -629,14 +643,14 @@
       <c r="A11" s="6">
         <v>2379581.0</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>43</v>
-      </c>
       <c s="7" t="s">
         <v>44</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>45</v>
+      </c>
+      <c s="8" t="s">
+        <v>46</v>
       </c>
       <c s="8" t="s">
         <v>14</v>
@@ -652,13 +666,10 @@
       <c r="A12" s="3">
         <v>3660603.0</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>46</v>
-      </c>
       <c s="4" t="s">
         <v>47</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>48</v>
       </c>
       <c s="5" t="s">
@@ -666,6 +677,9 @@
       </c>
       <c s="5" t="s">
         <v>50</v>
+      </c>
+      <c s="5" t="s">
+        <v>51</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -675,20 +689,20 @@
       <c r="A13" s="6">
         <v>3660992.0</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>51</v>
-      </c>
       <c s="7" t="s">
         <v>52</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>53</v>
       </c>
       <c s="8" t="s">
+        <v>54</v>
+      </c>
+      <c s="8" t="s">
         <v>39</v>
       </c>
       <c s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -698,20 +712,20 @@
       <c r="A14" s="3">
         <v>4787165.0</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>55</v>
-      </c>
       <c s="4" t="s">
         <v>56</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>57</v>
       </c>
       <c s="5" t="s">
-        <v>50</v>
-      </c>
-      <c s="5" t="s">
         <v>58</v>
+      </c>
+      <c s="5" t="s">
+        <v>51</v>
+      </c>
+      <c s="5" t="s">
+        <v>59</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -721,17 +735,17 @@
       <c r="A15" s="6">
         <v>7701708.0</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c s="7" t="s">
+        <v>60</v>
+      </c>
+      <c s="7" t="s">
+        <v>61</v>
+      </c>
+      <c s="8" t="s">
+        <v>62</v>
+      </c>
+      <c s="8" t="s">
         <v>59</v>
-      </c>
-      <c s="7" t="s">
-        <v>60</v>
-      </c>
-      <c s="8" t="s">
-        <v>61</v>
-      </c>
-      <c s="8" t="s">
-        <v>58</v>
       </c>
       <c s="8" t="s">
         <v>9</v>
@@ -744,17 +758,17 @@
       <c r="A16" s="3">
         <v>53161.0</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>62</v>
-      </c>
       <c s="4" t="s">
         <v>63</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>64</v>
       </c>
       <c s="5" t="s">
-        <v>58</v>
+        <v>65</v>
+      </c>
+      <c s="5" t="s">
+        <v>30</v>
       </c>
       <c s="5" t="s">
         <v>9</v>
@@ -767,20 +781,20 @@
       <c r="A17" s="6">
         <v>4548474.0</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>65</v>
-      </c>
       <c s="7" t="s">
         <v>66</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>67</v>
       </c>
       <c s="8" t="s">
-        <v>50</v>
-      </c>
-      <c s="8" t="s">
-        <v>58</v>
+        <v>68</v>
+      </c>
+      <c s="8" t="s">
+        <v>51</v>
+      </c>
+      <c s="8" t="s">
+        <v>59</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -790,20 +804,20 @@
       <c r="A18" s="3">
         <v>3661029.0</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>68</v>
-      </c>
       <c s="4" t="s">
         <v>69</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>70</v>
       </c>
       <c s="5" t="s">
+        <v>71</v>
+      </c>
+      <c s="5" t="s">
         <v>15</v>
       </c>
       <c s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -813,14 +827,14 @@
       <c r="A19" s="6">
         <v>3661053.0</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>72</v>
-      </c>
       <c s="7" t="s">
         <v>73</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>74</v>
+      </c>
+      <c s="8" t="s">
+        <v>75</v>
       </c>
       <c s="8" t="s">
         <v>35</v>
@@ -836,14 +850,14 @@
       <c r="A20" s="3">
         <v>3661061.0</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>75</v>
-      </c>
       <c s="4" t="s">
         <v>76</v>
       </c>
-      <c s="5" t="s">
+      <c s="4" t="s">
         <v>77</v>
+      </c>
+      <c s="5" t="s">
+        <v>78</v>
       </c>
       <c s="5" t="s">
         <v>23</v>
@@ -857,26 +871,26 @@
     </row>
     <row r="21" ht="17.0" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C21" s="9">
         <v>19.0</v>
       </c>
     </row>
     <row r="22" ht="17.0" customHeight="1">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c s="13">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23" ht="17.0" customHeight="1">
+      <c r="A23" s="12" t="s">
         <v>80</v>
       </c>
-      <c s="9">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="23" ht="17.0" customHeight="1">
-      <c r="A23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="11">
-        <v>43959.12503472222</v>
+      <c r="C23" s="11">
+        <v>43963.125023148146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First commit from vs code
</commit_message>
<xml_diff>
--- a/Handicap Index Course Handicap Report.xlsx
+++ b/Handicap Index Course Handicap Report.xlsx
@@ -37,7 +37,7 @@
     <t>Reid Baker</t>
   </si>
   <si>
-    <t>11.8</t>
+    <t>11.9</t>
   </si>
   <si>
     <t>12</t>
@@ -67,7 +67,10 @@
     <t>Rick Baumgarth</t>
   </si>
   <si>
-    <t>11.7</t>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>Besse</t>
@@ -76,6 +79,15 @@
     <t>Rick Besse</t>
   </si>
   <si>
+    <t>14.0</t>
+  </si>
+  <si>
+    <t>Broyles</t>
+  </si>
+  <si>
+    <t>Frank Broyles</t>
+  </si>
+  <si>
     <t>15.2</t>
   </si>
   <si>
@@ -85,37 +97,25 @@
     <t>18</t>
   </si>
   <si>
-    <t>Broyles</t>
-  </si>
-  <si>
-    <t>Frank Broyles</t>
-  </si>
-  <si>
-    <t>15.4</t>
-  </si>
-  <si>
     <t>Carroll</t>
   </si>
   <si>
     <t>Jack Carroll</t>
   </si>
   <si>
-    <t>9.5</t>
+    <t>9.3</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Davis</t>
   </si>
   <si>
     <t>Will Davis</t>
   </si>
   <si>
-    <t>14.7</t>
+    <t>14.4</t>
   </si>
   <si>
     <t>15</t>
@@ -139,7 +139,7 @@
     <t>Kent Fannon</t>
   </si>
   <si>
-    <t>13.4</t>
+    <t>13.0</t>
   </si>
   <si>
     <t>13</t>
@@ -160,36 +160,39 @@
     <t>Bob Heard</t>
   </si>
   <si>
-    <t>6.9</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Humphrey</t>
+  </si>
+  <si>
+    <t>Richard Humphrey</t>
+  </si>
+  <si>
+    <t>18.2</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Sido</t>
+  </si>
+  <si>
+    <t>Jim Sido</t>
+  </si>
+  <si>
+    <t>8.2</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>Humphrey</t>
-  </si>
-  <si>
-    <t>Richard Humphrey</t>
-  </si>
-  <si>
-    <t>18.3</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Sido</t>
-  </si>
-  <si>
-    <t>Jim Sido</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -199,9 +202,6 @@
     <t>Dan Stewart</t>
   </si>
   <si>
-    <t>10.3</t>
-  </si>
-  <si>
     <t>Strand</t>
   </si>
   <si>
@@ -217,7 +217,7 @@
     <t>Larry Traub</t>
   </si>
   <si>
-    <t>8.5</t>
+    <t>9.0</t>
   </si>
   <si>
     <t>Vela</t>
@@ -226,10 +226,10 @@
     <t>Al Vela</t>
   </si>
   <si>
-    <t>19.4</t>
-  </si>
-  <si>
-    <t>23</t>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
   <si>
     <t>Wickham</t>
@@ -238,7 +238,7 @@
     <t>Jimmy Wickham</t>
   </si>
   <si>
-    <t>14.9</t>
+    <t>14.5</t>
   </si>
   <si>
     <t>Williams</t>
@@ -247,7 +247,7 @@
     <t>Doug Williams</t>
   </si>
   <si>
-    <t>17.1</t>
+    <t>16.3</t>
   </si>
   <si>
     <t>Total Golfers:</t>
@@ -492,7 +492,7 @@
         <v>18</v>
       </c>
       <c s="5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c s="5" t="s">
         <v>10</v>
@@ -506,19 +506,19 @@
         <v>3660283.0</v>
       </c>
       <c s="7" t="s">
-        <v>19</v>
-      </c>
-      <c s="7" t="s">
         <v>20</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>21</v>
       </c>
       <c s="8" t="s">
         <v>22</v>
       </c>
       <c s="8" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c s="8" t="s">
+        <v>14</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -529,19 +529,19 @@
         <v>2379621.0</v>
       </c>
       <c s="4" t="s">
+        <v>23</v>
+      </c>
+      <c s="4" t="s">
         <v>24</v>
       </c>
-      <c s="4" t="s">
+      <c s="5" t="s">
         <v>25</v>
       </c>
       <c s="5" t="s">
         <v>26</v>
       </c>
       <c s="5" t="s">
-        <v>22</v>
-      </c>
-      <c s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -552,12 +552,9 @@
         <v>3660366.0</v>
       </c>
       <c s="7" t="s">
-        <v>27</v>
-      </c>
-      <c s="7" t="s">
         <v>28</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>29</v>
       </c>
       <c s="8" t="s">
@@ -565,6 +562,9 @@
       </c>
       <c s="8" t="s">
         <v>31</v>
+      </c>
+      <c s="8" t="s">
+        <v>19</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -587,7 +587,7 @@
         <v>35</v>
       </c>
       <c s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -633,7 +633,7 @@
         <v>43</v>
       </c>
       <c s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -722,10 +722,10 @@
         <v>58</v>
       </c>
       <c s="5" t="s">
-        <v>51</v>
-      </c>
-      <c s="5" t="s">
         <v>59</v>
+      </c>
+      <c s="5" t="s">
+        <v>60</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -736,19 +736,19 @@
         <v>7701708.0</v>
       </c>
       <c s="7" t="s">
-        <v>60</v>
-      </c>
-      <c s="7" t="s">
         <v>61</v>
       </c>
-      <c s="8" t="s">
+      <c s="7" t="s">
         <v>62</v>
       </c>
       <c s="8" t="s">
-        <v>59</v>
-      </c>
-      <c s="8" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c s="8" t="s">
+        <v>31</v>
+      </c>
+      <c s="8" t="s">
+        <v>19</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -768,7 +768,7 @@
         <v>65</v>
       </c>
       <c s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c s="5" t="s">
         <v>9</v>
@@ -791,10 +791,10 @@
         <v>68</v>
       </c>
       <c s="8" t="s">
-        <v>51</v>
-      </c>
-      <c s="8" t="s">
         <v>59</v>
+      </c>
+      <c s="8" t="s">
+        <v>19</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -814,7 +814,7 @@
         <v>71</v>
       </c>
       <c s="5" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c s="5" t="s">
         <v>72</v>
@@ -840,7 +840,7 @@
         <v>35</v>
       </c>
       <c s="8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c s="8"/>
       <c s="8"/>
@@ -860,10 +860,10 @@
         <v>78</v>
       </c>
       <c s="5" t="s">
-        <v>23</v>
-      </c>
-      <c s="5" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c s="5" t="s">
+        <v>39</v>
       </c>
       <c s="5"/>
       <c s="5"/>
@@ -890,7 +890,7 @@
         <v>80</v>
       </c>
       <c r="C23" s="11">
-        <v>43963.125023148146</v>
+        <v>43979.12501157408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>